<commit_message>
Simplify build script optimization
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1409,6 +1409,43 @@
         <v>376</v>
       </c>
       <c r="I26" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45813.43701388889</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0x01,0x78</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>380</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>376</v>
+      </c>
+      <c r="I27" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1423,7 +1460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2400,6 +2437,43 @@
         <v>376</v>
       </c>
       <c r="I26" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45813.43701388889</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0x01,0x78</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>380</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>376</v>
+      </c>
+      <c r="I27" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2414,7 +2488,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3391,6 +3465,43 @@
         <v>130</v>
       </c>
       <c r="I26" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45813.43701388889</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>130</v>
+      </c>
+      <c r="G27" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>130</v>
+      </c>
+      <c r="I27" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3405,7 +3516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4385,6 +4496,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>45813.43701388889</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0x00,0x81</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>130</v>
+      </c>
+      <c r="G27" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H27" t="n">
+        <v>129</v>
+      </c>
+      <c r="I27" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize user authentication module
Improve performance by optimizing database queries.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1557,6 +1557,43 @@
         <v>376</v>
       </c>
       <c r="I30" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45817.43892361111</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x01,0x78</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>380</v>
+      </c>
+      <c r="G31" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H31" t="n">
+        <v>376</v>
+      </c>
+      <c r="I31" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1571,7 +1608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2696,6 +2733,43 @@
         <v>376</v>
       </c>
       <c r="I30" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45817.43892361111</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x01,0x78</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>380</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H31" t="n">
+        <v>376</v>
+      </c>
+      <c r="I31" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2710,7 +2784,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3835,6 +3909,43 @@
         <v>129</v>
       </c>
       <c r="I30" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45817.43892361111</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>130</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H31" t="n">
+        <v>129</v>
+      </c>
+      <c r="I31" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3849,7 +3960,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4977,6 +5088,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>45817.43892361111</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0x00,0x81</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>130</v>
+      </c>
+      <c r="G31" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H31" t="n">
+        <v>129</v>
+      </c>
+      <c r="I31" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize image processing memory leaks
Apply code style fixes as per linter recommendations.
Add input validation for better security.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1964,6 +1964,43 @@
         <v>364</v>
       </c>
       <c r="I41" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45828.43628472222</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0x01,0x6C</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>380</v>
+      </c>
+      <c r="G42" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H42" t="n">
+        <v>364</v>
+      </c>
+      <c r="I42" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1978,7 +2015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3510,6 +3547,43 @@
         <v>364</v>
       </c>
       <c r="I41" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45828.43628472222</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0x01,0x6C</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>380</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H42" t="n">
+        <v>364</v>
+      </c>
+      <c r="I42" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3524,7 +3598,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5056,6 +5130,43 @@
         <v>127</v>
       </c>
       <c r="I41" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45828.43628472222</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0x00,0x7F</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>130</v>
+      </c>
+      <c r="G42" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H42" t="n">
+        <v>127</v>
+      </c>
+      <c r="I42" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5070,7 +5181,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6605,6 +6716,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>45828.43628472222</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0x00,0x7F</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>130</v>
+      </c>
+      <c r="G42" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H42" t="n">
+        <v>127</v>
+      </c>
+      <c r="I42" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjust api response formatting
Fix various typos in comments and documentation.
This resolves issue #17.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2038,6 +2038,43 @@
         <v>360</v>
       </c>
       <c r="I43" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>45830.43821759259</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0x01,0x68</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>380</v>
+      </c>
+      <c r="G44" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H44" t="n">
+        <v>360</v>
+      </c>
+      <c r="I44" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2052,7 +2089,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3658,6 +3695,43 @@
         <v>360</v>
       </c>
       <c r="I43" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>45830.43821759259</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0x01,0x68</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>380</v>
+      </c>
+      <c r="G44" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H44" t="n">
+        <v>360</v>
+      </c>
+      <c r="I44" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3672,7 +3746,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5278,6 +5352,43 @@
         <v>127</v>
       </c>
       <c r="I43" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>45830.43821759259</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0x00,0x7F</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>130</v>
+      </c>
+      <c r="G44" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H44" t="n">
+        <v>127</v>
+      </c>
+      <c r="I44" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5292,7 +5403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6901,6 +7012,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>45830.43821759259</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0x00,0x7F</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>130</v>
+      </c>
+      <c r="G44" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H44" t="n">
+        <v>127</v>
+      </c>
+      <c r="I44" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert config file handling
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2075,6 +2075,43 @@
         <v>360</v>
       </c>
       <c r="I44" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45831.43658564815</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x01,0x68</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>380</v>
+      </c>
+      <c r="G45" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H45" t="n">
+        <v>360</v>
+      </c>
+      <c r="I45" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2089,7 +2126,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3732,6 +3769,43 @@
         <v>360</v>
       </c>
       <c r="I44" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45831.43658564815</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x01,0x68</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>380</v>
+      </c>
+      <c r="G45" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H45" t="n">
+        <v>360</v>
+      </c>
+      <c r="I45" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3746,7 +3820,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5389,6 +5463,43 @@
         <v>127</v>
       </c>
       <c r="I44" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45831.43658564815</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x00,0x7F</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>130</v>
+      </c>
+      <c r="G45" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H45" t="n">
+        <v>127</v>
+      </c>
+      <c r="I45" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5403,7 +5514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7049,6 +7160,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>45831.43658564815</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0x00,0x7F</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>130</v>
+      </c>
+      <c r="G45" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H45" t="n">
+        <v>127</v>
+      </c>
+      <c r="I45" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix login page ui elements
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2186,6 +2186,43 @@
         <v>356</v>
       </c>
       <c r="I47" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45834.43858796296</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x01,0x64</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>380</v>
+      </c>
+      <c r="G48" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H48" t="n">
+        <v>356</v>
+      </c>
+      <c r="I48" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2200,7 +2237,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3954,6 +3991,43 @@
         <v>360</v>
       </c>
       <c r="I47" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45834.43858796296</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x01,0x64</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>380</v>
+      </c>
+      <c r="G48" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H48" t="n">
+        <v>356</v>
+      </c>
+      <c r="I48" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3968,7 +4042,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5722,6 +5796,43 @@
         <v>127</v>
       </c>
       <c r="I47" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45834.43858796296</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x00,0x7F</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>130</v>
+      </c>
+      <c r="G48" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H48" t="n">
+        <v>127</v>
+      </c>
+      <c r="I48" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5736,7 +5847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7493,6 +7604,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>45834.43858796296</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0x00,0x7E</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>130</v>
+      </c>
+      <c r="G48" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H48" t="n">
+        <v>126</v>
+      </c>
+      <c r="I48" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improve file upload functionality
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2223,6 +2223,43 @@
         <v>356</v>
       </c>
       <c r="I48" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45835.43721064815</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x01,0x64</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>380</v>
+      </c>
+      <c r="G49" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H49" t="n">
+        <v>356</v>
+      </c>
+      <c r="I49" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2237,7 +2274,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4028,6 +4065,43 @@
         <v>356</v>
       </c>
       <c r="I48" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45835.43721064815</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x01,0x64</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>380</v>
+      </c>
+      <c r="G49" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H49" t="n">
+        <v>356</v>
+      </c>
+      <c r="I49" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4042,7 +4116,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5833,6 +5907,43 @@
         <v>127</v>
       </c>
       <c r="I48" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45835.43721064815</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x00,0x7F</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>130</v>
+      </c>
+      <c r="G49" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H49" t="n">
+        <v>127</v>
+      </c>
+      <c r="I49" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5847,7 +5958,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7641,6 +7752,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>45835.43721064815</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>0x00,0x7E</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>130</v>
+      </c>
+      <c r="G49" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H49" t="n">
+        <v>126</v>
+      </c>
+      <c r="I49" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add image processing memory leaks
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2260,6 +2260,43 @@
         <v>356</v>
       </c>
       <c r="I49" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>45836.43600694444</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0x01,0x64</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>380</v>
+      </c>
+      <c r="G50" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H50" t="n">
+        <v>356</v>
+      </c>
+      <c r="I50" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2274,7 +2311,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4102,6 +4139,43 @@
         <v>356</v>
       </c>
       <c r="I49" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>45836.43600694444</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0x01,0x64</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>380</v>
+      </c>
+      <c r="G50" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H50" t="n">
+        <v>356</v>
+      </c>
+      <c r="I50" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4116,7 +4190,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5944,6 +6018,43 @@
         <v>127</v>
       </c>
       <c r="I49" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>45836.43600694444</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0x00,0x7F</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>130</v>
+      </c>
+      <c r="G50" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H50" t="n">
+        <v>127</v>
+      </c>
+      <c r="I50" t="n">
         <v>7</v>
       </c>
     </row>
@@ -5958,7 +6069,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7789,6 +7900,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>45836.43600694444</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>0x00,0x7E</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>130</v>
+      </c>
+      <c r="G50" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H50" t="n">
+        <v>126</v>
+      </c>
+      <c r="I50" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor api response formatting
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2297,6 +2297,43 @@
         <v>356</v>
       </c>
       <c r="I50" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45837.43663194445</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x01,0x64</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>380</v>
+      </c>
+      <c r="G51" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H51" t="n">
+        <v>356</v>
+      </c>
+      <c r="I51" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2311,7 +2348,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4176,6 +4213,43 @@
         <v>356</v>
       </c>
       <c r="I50" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45837.43663194445</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x01,0x64</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>380</v>
+      </c>
+      <c r="G51" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H51" t="n">
+        <v>356</v>
+      </c>
+      <c r="I51" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4190,7 +4264,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6055,6 +6129,43 @@
         <v>127</v>
       </c>
       <c r="I50" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45837.43663194445</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x00,0x7E</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>130</v>
+      </c>
+      <c r="G51" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H51" t="n">
+        <v>126</v>
+      </c>
+      <c r="I51" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6069,7 +6180,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7937,6 +8048,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>45837.43663194445</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0x00,0x7E</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>130</v>
+      </c>
+      <c r="G51" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H51" t="n">
+        <v>126</v>
+      </c>
+      <c r="I51" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor image processing memory leaks
Optimize image compression algorithm.
Improve performance by optimizing database queries.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2482,6 +2482,43 @@
         <v>352</v>
       </c>
       <c r="I55" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45842.43524305556</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x01,0x60</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>380</v>
+      </c>
+      <c r="G56" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H56" t="n">
+        <v>352</v>
+      </c>
+      <c r="I56" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2496,7 +2533,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4546,6 +4583,43 @@
         <v>352</v>
       </c>
       <c r="I55" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45842.43524305556</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x01,0x60</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>380</v>
+      </c>
+      <c r="G56" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H56" t="n">
+        <v>352</v>
+      </c>
+      <c r="I56" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4560,7 +4634,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6610,6 +6684,43 @@
         <v>126</v>
       </c>
       <c r="I55" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45842.43524305556</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x00,0x7E</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>130</v>
+      </c>
+      <c r="G56" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H56" t="n">
+        <v>126</v>
+      </c>
+      <c r="I56" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6624,7 +6735,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8677,6 +8788,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>45842.43524305556</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>0x00,0x7D</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>130</v>
+      </c>
+      <c r="G56" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H56" t="n">
+        <v>125</v>
+      </c>
+      <c r="I56" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert file upload functionality
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2593,6 +2593,43 @@
         <v>348</v>
       </c>
       <c r="I58" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45845.43280092593</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x01,0x5C</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>380</v>
+      </c>
+      <c r="G59" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H59" t="n">
+        <v>348</v>
+      </c>
+      <c r="I59" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2607,7 +2644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4768,6 +4805,43 @@
         <v>352</v>
       </c>
       <c r="I58" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45845.43280092593</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x01,0x60</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>380</v>
+      </c>
+      <c r="G59" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H59" t="n">
+        <v>352</v>
+      </c>
+      <c r="I59" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4782,7 +4856,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6943,6 +7017,43 @@
         <v>126</v>
       </c>
       <c r="I58" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45845.43280092593</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x00,0x7E</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>130</v>
+      </c>
+      <c r="G59" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H59" t="n">
+        <v>126</v>
+      </c>
+      <c r="I59" t="n">
         <v>7</v>
       </c>
     </row>
@@ -6957,7 +7068,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9121,6 +9232,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45845.43280092593</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>0x00,0x7D</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>130</v>
+      </c>
+      <c r="G59" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H59" t="n">
+        <v>125</v>
+      </c>
+      <c r="I59" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance config file handling
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2667,6 +2667,43 @@
         <v>348</v>
       </c>
       <c r="I60" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45847.43748842592</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x01,0x5C</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>380</v>
+      </c>
+      <c r="G61" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H61" t="n">
+        <v>348</v>
+      </c>
+      <c r="I61" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2681,7 +2718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4916,6 +4953,43 @@
         <v>348</v>
       </c>
       <c r="I60" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45847.43748842592</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x01,0x5C</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>380</v>
+      </c>
+      <c r="G61" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H61" t="n">
+        <v>348</v>
+      </c>
+      <c r="I61" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4930,7 +5004,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7165,6 +7239,43 @@
         <v>126</v>
       </c>
       <c r="I60" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45847.43748842592</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x00,0x7D</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>130</v>
+      </c>
+      <c r="G61" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H61" t="n">
+        <v>125</v>
+      </c>
+      <c r="I61" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7179,7 +7290,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9417,6 +9528,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45847.43748842592</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>0x00,0x7D</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>130</v>
+      </c>
+      <c r="G61" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H61" t="n">
+        <v>125</v>
+      </c>
+      <c r="I61" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Correct csv module error handling
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2704,6 +2704,117 @@
         <v>348</v>
       </c>
       <c r="I61" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>45848.43368055556</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0x01,0x58</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>380</v>
+      </c>
+      <c r="G62" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H62" t="n">
+        <v>344</v>
+      </c>
+      <c r="I62" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>45849.43524305556</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0x01,0x58</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>380</v>
+      </c>
+      <c r="G63" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H63" t="n">
+        <v>344</v>
+      </c>
+      <c r="I63" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>45850.43918981482</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0x01,0x54</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>380</v>
+      </c>
+      <c r="G64" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H64" t="n">
+        <v>340</v>
+      </c>
+      <c r="I64" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2718,7 +2829,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4990,6 +5101,117 @@
         <v>348</v>
       </c>
       <c r="I61" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>45848.43368055556</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0x01,0x58</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>380</v>
+      </c>
+      <c r="G62" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H62" t="n">
+        <v>344</v>
+      </c>
+      <c r="I62" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>45849.43524305556</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0x01,0x58</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>380</v>
+      </c>
+      <c r="G63" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H63" t="n">
+        <v>344</v>
+      </c>
+      <c r="I63" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>45850.43918981482</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0x01,0x54</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>380</v>
+      </c>
+      <c r="G64" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H64" t="n">
+        <v>340</v>
+      </c>
+      <c r="I64" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5004,7 +5226,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6037,7 +6259,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0x00,0x82</t>
+          <t>0x00,0x81</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -6074,7 +6296,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0x00,0x82</t>
+          <t>0x00,0x81</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -6111,7 +6333,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0x00,0x82</t>
+          <t>0x00,0x81</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -6148,7 +6370,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0x00,0x82</t>
+          <t>0x00,0x81</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -6185,7 +6407,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0x00,0x82</t>
+          <t>0x00,0x81</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -6222,7 +6444,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0x00,0x82</t>
+          <t>0x00,0x81</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -6259,7 +6481,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0x00,0x80</t>
+          <t>0x00,0x81</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -6274,7 +6496,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H34" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I34" t="n">
         <v>7</v>
@@ -6740,7 +6962,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0x00,0x7F</t>
+          <t>0x00,0x7E</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -6755,7 +6977,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H47" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I47" t="n">
         <v>7</v>
@@ -6777,7 +6999,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0x00,0x7F</t>
+          <t>0x00,0x7E</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -6792,7 +7014,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H48" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I48" t="n">
         <v>7</v>
@@ -6814,7 +7036,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0x00,0x7F</t>
+          <t>0x00,0x7E</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -6829,7 +7051,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H49" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I49" t="n">
         <v>7</v>
@@ -6851,7 +7073,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0x00,0x7F</t>
+          <t>0x00,0x7E</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -6866,7 +7088,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H50" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I50" t="n">
         <v>7</v>
@@ -7073,7 +7295,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0x00,0x7E</t>
+          <t>0x00,0x7D</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -7088,7 +7310,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H56" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I56" t="n">
         <v>7</v>
@@ -7110,7 +7332,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0x00,0x7E</t>
+          <t>0x00,0x7D</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -7125,7 +7347,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H57" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I57" t="n">
         <v>7</v>
@@ -7147,7 +7369,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0x00,0x7E</t>
+          <t>0x00,0x7D</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -7162,7 +7384,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H58" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I58" t="n">
         <v>7</v>
@@ -7184,7 +7406,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0x00,0x7E</t>
+          <t>0x00,0x7D</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -7199,7 +7421,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H59" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I59" t="n">
         <v>7</v>
@@ -7221,7 +7443,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0x00,0x7E</t>
+          <t>0x00,0x7D</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -7236,7 +7458,7 @@
         <v>5.68631262647114e+23</v>
       </c>
       <c r="H60" t="n">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I60" t="n">
         <v>7</v>
@@ -7276,6 +7498,117 @@
         <v>125</v>
       </c>
       <c r="I61" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>45848.43368055556</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0x00,0x7C</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>130</v>
+      </c>
+      <c r="G62" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H62" t="n">
+        <v>124</v>
+      </c>
+      <c r="I62" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>45849.43524305556</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0x00,0x7C</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>130</v>
+      </c>
+      <c r="G63" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H63" t="n">
+        <v>124</v>
+      </c>
+      <c r="I63" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>45850.43918981482</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0x00,0x7C</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>130</v>
+      </c>
+      <c r="G64" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H64" t="n">
+        <v>124</v>
+      </c>
+      <c r="I64" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7290,7 +7623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8323,7 +8656,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0x00,0x81</t>
+          <t>0x00,0x82</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -8360,7 +8693,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0x00,0x81</t>
+          <t>0x00,0x82</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -8397,7 +8730,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0x00,0x81</t>
+          <t>0x00,0x82</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -8434,7 +8767,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0x00,0x81</t>
+          <t>0x00,0x82</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -8471,7 +8804,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0x00,0x81</t>
+          <t>0x00,0x82</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -8508,7 +8841,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0x00,0x81</t>
+          <t>0x00,0x82</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -8545,7 +8878,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0x00,0x81</t>
+          <t>0x00,0x80</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -8560,7 +8893,7 @@
         <v>9.85046333984776e+23</v>
       </c>
       <c r="H34" t="n">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I34" t="n">
         <v>3</v>
@@ -9026,7 +9359,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>0x00,0x7E</t>
+          <t>0x00,0x7F</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -9041,7 +9374,7 @@
         <v>9.85046333984776e+23</v>
       </c>
       <c r="H47" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I47" t="n">
         <v>3</v>
@@ -9063,7 +9396,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>0x00,0x7E</t>
+          <t>0x00,0x7F</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -9078,7 +9411,7 @@
         <v>9.85046333984776e+23</v>
       </c>
       <c r="H48" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I48" t="n">
         <v>3</v>
@@ -9100,7 +9433,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>0x00,0x7E</t>
+          <t>0x00,0x7F</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -9115,7 +9448,7 @@
         <v>9.85046333984776e+23</v>
       </c>
       <c r="H49" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I49" t="n">
         <v>3</v>
@@ -9137,7 +9470,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>0x00,0x7E</t>
+          <t>0x00,0x7F</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -9152,7 +9485,7 @@
         <v>9.85046333984776e+23</v>
       </c>
       <c r="H50" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I50" t="n">
         <v>3</v>
@@ -9359,7 +9692,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>0x00,0x7D</t>
+          <t>0x00,0x7E</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -9374,7 +9707,7 @@
         <v>9.85046333984776e+23</v>
       </c>
       <c r="H56" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I56" t="n">
         <v>3</v>
@@ -9396,7 +9729,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0x00,0x7D</t>
+          <t>0x00,0x7E</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -9411,7 +9744,7 @@
         <v>9.85046333984776e+23</v>
       </c>
       <c r="H57" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I57" t="n">
         <v>3</v>
@@ -9433,7 +9766,7 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>0x00,0x7D</t>
+          <t>0x00,0x7E</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -9448,7 +9781,7 @@
         <v>9.85046333984776e+23</v>
       </c>
       <c r="H58" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I58" t="n">
         <v>3</v>
@@ -9470,7 +9803,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0x00,0x7D</t>
+          <t>0x00,0x7E</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -9485,7 +9818,7 @@
         <v>9.85046333984776e+23</v>
       </c>
       <c r="H59" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I59" t="n">
         <v>3</v>
@@ -9507,7 +9840,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>0x00,0x7D</t>
+          <t>0x00,0x7E</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -9522,7 +9855,7 @@
         <v>9.85046333984776e+23</v>
       </c>
       <c r="H60" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I60" t="n">
         <v>3</v>
@@ -9562,6 +9895,117 @@
         <v>125</v>
       </c>
       <c r="I61" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>45848.43368055556</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>0x00,0x7C</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>130</v>
+      </c>
+      <c r="G62" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H62" t="n">
+        <v>124</v>
+      </c>
+      <c r="I62" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>45849.43524305556</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>0x00,0x7C</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>130</v>
+      </c>
+      <c r="G63" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H63" t="n">
+        <v>124</v>
+      </c>
+      <c r="I63" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>45850.43918981482</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>0x00,0x7C</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>130</v>
+      </c>
+      <c r="G64" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H64" t="n">
+        <v>124</v>
+      </c>
+      <c r="I64" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement navigation menu accessibility
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2852,6 +2852,43 @@
         <v>340</v>
       </c>
       <c r="I65" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>45852.43335648148</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0x01,0x50</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>380</v>
+      </c>
+      <c r="G66" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H66" t="n">
+        <v>336</v>
+      </c>
+      <c r="I66" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2866,7 +2903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5286,6 +5323,43 @@
         <v>340</v>
       </c>
       <c r="I65" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>45852.43335648148</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0x01,0x50</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>380</v>
+      </c>
+      <c r="G66" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H66" t="n">
+        <v>336</v>
+      </c>
+      <c r="I66" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5300,7 +5374,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7720,6 +7794,43 @@
         <v>124</v>
       </c>
       <c r="I65" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>45852.43335648148</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0x00,0x7B</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>130</v>
+      </c>
+      <c r="G66" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H66" t="n">
+        <v>123</v>
+      </c>
+      <c r="I66" t="n">
         <v>7</v>
       </c>
     </row>
@@ -7734,7 +7845,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10157,6 +10268,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>45852.43335648148</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>0x00,0x7B</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>130</v>
+      </c>
+      <c r="G66" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H66" t="n">
+        <v>123</v>
+      </c>
+      <c r="I66" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjust responsive design implementation
This resolves issue #74.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2963,6 +2963,43 @@
         <v>332</v>
       </c>
       <c r="I68" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45855.43355324074</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x01,0x4C</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>380</v>
+      </c>
+      <c r="G69" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H69" t="n">
+        <v>332</v>
+      </c>
+      <c r="I69" t="n">
         <v>14</v>
       </c>
     </row>
@@ -2977,7 +3014,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5508,6 +5545,43 @@
         <v>336</v>
       </c>
       <c r="I68" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45855.43355324074</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x01,0x4C</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>380</v>
+      </c>
+      <c r="G69" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H69" t="n">
+        <v>332</v>
+      </c>
+      <c r="I69" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5522,7 +5596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8053,6 +8127,43 @@
         <v>123</v>
       </c>
       <c r="I68" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45855.43355324074</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x00,0x7A</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>130</v>
+      </c>
+      <c r="G69" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H69" t="n">
+        <v>122</v>
+      </c>
+      <c r="I69" t="n">
         <v>7</v>
       </c>
     </row>
@@ -8067,7 +8178,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10601,6 +10712,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>45855.43355324074</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>0x00,0x7A</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>130</v>
+      </c>
+      <c r="G69" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H69" t="n">
+        <v>122</v>
+      </c>
+      <c r="I69" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update logging system configuration
Remove deprecated functions and clean up codebase.
Fix race condition in concurrent processing.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3074,6 +3074,43 @@
         <v>328</v>
       </c>
       <c r="I71" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45858.43453703704</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0x01,0x48</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>380</v>
+      </c>
+      <c r="G72" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H72" t="n">
+        <v>328</v>
+      </c>
+      <c r="I72" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3088,7 +3125,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5730,6 +5767,43 @@
         <v>328</v>
       </c>
       <c r="I71" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45858.43453703704</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0x01,0x48</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>380</v>
+      </c>
+      <c r="G72" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H72" t="n">
+        <v>328</v>
+      </c>
+      <c r="I72" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5744,7 +5818,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8386,6 +8460,43 @@
         <v>122</v>
       </c>
       <c r="I71" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45858.43453703704</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0x00,0x7A</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>130</v>
+      </c>
+      <c r="G72" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H72" t="n">
+        <v>122</v>
+      </c>
+      <c r="I72" t="n">
         <v>7</v>
       </c>
     </row>
@@ -8400,7 +8511,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11045,6 +11156,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>45858.43453703704</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>0x00,0x7A</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>130</v>
+      </c>
+      <c r="G72" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H72" t="n">
+        <v>122</v>
+      </c>
+      <c r="I72" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upgrade navigation menu accessibility
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3518,6 +3518,43 @@
         <v>308</v>
       </c>
       <c r="I83" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45870.43944444445</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0x01,0x34</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>380</v>
+      </c>
+      <c r="G84" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H84" t="n">
+        <v>308</v>
+      </c>
+      <c r="I84" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3532,7 +3569,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6618,6 +6655,43 @@
         <v>312</v>
       </c>
       <c r="I83" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45870.43944444445</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0x01,0x38</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>380</v>
+      </c>
+      <c r="G84" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H84" t="n">
+        <v>312</v>
+      </c>
+      <c r="I84" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6632,7 +6706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9718,6 +9792,43 @@
         <v>119</v>
       </c>
       <c r="I83" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45870.43944444445</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0x00,0x77</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>130</v>
+      </c>
+      <c r="G84" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H84" t="n">
+        <v>119</v>
+      </c>
+      <c r="I84" t="n">
         <v>7</v>
       </c>
     </row>
@@ -9732,7 +9843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12821,6 +12932,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>45870.43944444445</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>0x00,0x76</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F84" t="n">
+        <v>130</v>
+      </c>
+      <c r="G84" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H84" t="n">
+        <v>118</v>
+      </c>
+      <c r="I84" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjust logging system configuration
Apply code style fixes as per linter recommendations.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3629,6 +3629,43 @@
         <v>308</v>
       </c>
       <c r="I86" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45873.43682870371</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0x01,0x34</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>380</v>
+      </c>
+      <c r="G87" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H87" t="n">
+        <v>308</v>
+      </c>
+      <c r="I87" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3643,7 +3680,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6840,6 +6877,43 @@
         <v>312</v>
       </c>
       <c r="I86" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45873.43682870371</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0x01,0x34</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>380</v>
+      </c>
+      <c r="G87" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H87" t="n">
+        <v>308</v>
+      </c>
+      <c r="I87" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6854,7 +6928,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10051,6 +10125,43 @@
         <v>119</v>
       </c>
       <c r="I86" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45873.43682870371</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0x00,0x77</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>130</v>
+      </c>
+      <c r="G87" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H87" t="n">
+        <v>119</v>
+      </c>
+      <c r="I87" t="n">
         <v>7</v>
       </c>
     </row>
@@ -10065,7 +10176,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13265,6 +13376,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>45873.43682870371</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>0x00,0x75</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F87" t="n">
+        <v>130</v>
+      </c>
+      <c r="G87" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H87" t="n">
+        <v>117</v>
+      </c>
+      <c r="I87" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor csv module error handling
Add missing documentation for the new API.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3666,6 +3666,43 @@
         <v>308</v>
       </c>
       <c r="I87" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45874.43753472222</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0x01,0x30</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>380</v>
+      </c>
+      <c r="G88" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H88" t="n">
+        <v>304</v>
+      </c>
+      <c r="I88" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3680,7 +3717,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6914,6 +6951,43 @@
         <v>308</v>
       </c>
       <c r="I87" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45874.43753472222</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0x01,0x34</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>380</v>
+      </c>
+      <c r="G88" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H88" t="n">
+        <v>308</v>
+      </c>
+      <c r="I88" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6928,7 +7002,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10162,6 +10236,43 @@
         <v>119</v>
       </c>
       <c r="I87" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45874.43753472222</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0x00,0x76</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>130</v>
+      </c>
+      <c r="G88" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H88" t="n">
+        <v>118</v>
+      </c>
+      <c r="I88" t="n">
         <v>7</v>
       </c>
     </row>
@@ -10176,7 +10287,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13413,6 +13524,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>45874.43753472222</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>0x00,0x75</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F88" t="n">
+        <v>130</v>
+      </c>
+      <c r="G88" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H88" t="n">
+        <v>117</v>
+      </c>
+      <c r="I88" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance security vulnerability checks
Address edge cases reported in user feedback.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3703,6 +3703,43 @@
         <v>304</v>
       </c>
       <c r="I88" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45875.43287037037</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0x01,0x30</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>380</v>
+      </c>
+      <c r="G89" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H89" t="n">
+        <v>304</v>
+      </c>
+      <c r="I89" t="n">
         <v>14</v>
       </c>
     </row>
@@ -3717,7 +3754,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6988,6 +7025,43 @@
         <v>308</v>
       </c>
       <c r="I88" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45875.43287037037</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0x01,0x34</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>380</v>
+      </c>
+      <c r="G89" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H89" t="n">
+        <v>308</v>
+      </c>
+      <c r="I89" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7002,7 +7076,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10273,6 +10347,43 @@
         <v>118</v>
       </c>
       <c r="I88" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45875.43287037037</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0x00,0x76</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>130</v>
+      </c>
+      <c r="G89" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H89" t="n">
+        <v>118</v>
+      </c>
+      <c r="I89" t="n">
         <v>7</v>
       </c>
     </row>
@@ -10287,7 +10398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13561,6 +13672,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>45875.43287037037</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>0x00,0x75</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F89" t="n">
+        <v>130</v>
+      </c>
+      <c r="G89" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H89" t="n">
+        <v>117</v>
+      </c>
+      <c r="I89" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjust login page ui elements
Address edge cases reported in user feedback.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3999,6 +3999,43 @@
         <v>292</v>
       </c>
       <c r="I96" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>45883.43665509259</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>0x01,0x24</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>380</v>
+      </c>
+      <c r="G97" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H97" t="n">
+        <v>292</v>
+      </c>
+      <c r="I97" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4013,7 +4050,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7580,6 +7617,43 @@
         <v>300</v>
       </c>
       <c r="I96" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>45883.43665509259</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>0x01,0x28</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>380</v>
+      </c>
+      <c r="G97" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H97" t="n">
+        <v>296</v>
+      </c>
+      <c r="I97" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7594,7 +7668,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11161,6 +11235,43 @@
         <v>117</v>
       </c>
       <c r="I96" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>45883.43665509259</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>0x00,0x75</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>130</v>
+      </c>
+      <c r="G97" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H97" t="n">
+        <v>117</v>
+      </c>
+      <c r="I97" t="n">
         <v>7</v>
       </c>
     </row>
@@ -11175,7 +11286,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14745,6 +14856,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>45883.43665509259</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>0x00,0x74</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F97" t="n">
+        <v>130</v>
+      </c>
+      <c r="G97" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H97" t="n">
+        <v>116</v>
+      </c>
+      <c r="I97" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise api endpoint validation
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4221,6 +4221,43 @@
         <v>288</v>
       </c>
       <c r="I102" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45889.43734953704</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>0x01,0x20</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>380</v>
+      </c>
+      <c r="G103" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H103" t="n">
+        <v>288</v>
+      </c>
+      <c r="I103" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4235,7 +4272,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8024,6 +8061,43 @@
         <v>292</v>
       </c>
       <c r="I102" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45889.43734953704</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>0x01,0x24</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>380</v>
+      </c>
+      <c r="G103" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H103" t="n">
+        <v>292</v>
+      </c>
+      <c r="I103" t="n">
         <v>14</v>
       </c>
     </row>
@@ -8038,7 +8112,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11827,6 +11901,43 @@
         <v>116</v>
       </c>
       <c r="I102" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45889.43734953704</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>0x00,0x73</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>130</v>
+      </c>
+      <c r="G103" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H103" t="n">
+        <v>115</v>
+      </c>
+      <c r="I103" t="n">
         <v>7</v>
       </c>
     </row>
@@ -11841,7 +11952,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15633,6 +15744,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>45889.43734953704</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>0x00,0x72</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F103" t="n">
+        <v>130</v>
+      </c>
+      <c r="G103" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H103" t="n">
+        <v>114</v>
+      </c>
+      <c r="I103" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement login page ui elements
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4332,6 +4332,117 @@
         <v>284</v>
       </c>
       <c r="I105" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>45892.43943287037</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>0x01,0x1C</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>380</v>
+      </c>
+      <c r="G106" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H106" t="n">
+        <v>284</v>
+      </c>
+      <c r="I106" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>45893.43509259259</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0x01,0x1C</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>380</v>
+      </c>
+      <c r="G107" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H107" t="n">
+        <v>284</v>
+      </c>
+      <c r="I107" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>45894.438125</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0x01,0x1C</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>380</v>
+      </c>
+      <c r="G108" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H108" t="n">
+        <v>284</v>
+      </c>
+      <c r="I108" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4346,7 +4457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8246,6 +8357,117 @@
         <v>292</v>
       </c>
       <c r="I105" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>45892.43943287037</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>0x01,0x20</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>380</v>
+      </c>
+      <c r="G106" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H106" t="n">
+        <v>288</v>
+      </c>
+      <c r="I106" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>45893.43509259259</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0x01,0x20</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>380</v>
+      </c>
+      <c r="G107" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H107" t="n">
+        <v>288</v>
+      </c>
+      <c r="I107" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>45894.438125</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0x01,0x20</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>380</v>
+      </c>
+      <c r="G108" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H108" t="n">
+        <v>288</v>
+      </c>
+      <c r="I108" t="n">
         <v>14</v>
       </c>
     </row>
@@ -8260,7 +8482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12160,6 +12382,117 @@
         <v>115</v>
       </c>
       <c r="I105" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>45892.43943287037</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>0x00,0x73</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>130</v>
+      </c>
+      <c r="G106" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H106" t="n">
+        <v>115</v>
+      </c>
+      <c r="I106" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>45893.43509259259</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0x00,0x73</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>130</v>
+      </c>
+      <c r="G107" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H107" t="n">
+        <v>115</v>
+      </c>
+      <c r="I107" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>45894.438125</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0x00,0x73</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>130</v>
+      </c>
+      <c r="G108" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H108" t="n">
+        <v>115</v>
+      </c>
+      <c r="I108" t="n">
         <v>7</v>
       </c>
     </row>
@@ -12174,7 +12507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16077,6 +16410,117 @@
         <v>3</v>
       </c>
     </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>45892.43943287037</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>0x00,0x71</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>130</v>
+      </c>
+      <c r="G106" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H106" t="n">
+        <v>113</v>
+      </c>
+      <c r="I106" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>45893.43509259259</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>0x00,0x71</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>130</v>
+      </c>
+      <c r="G107" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H107" t="n">
+        <v>113</v>
+      </c>
+      <c r="I107" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>45894.438125</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>0x00,0x71</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F108" t="n">
+        <v>130</v>
+      </c>
+      <c r="G108" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H108" t="n">
+        <v>113</v>
+      </c>
+      <c r="I108" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor error message display
Improve performance by optimizing database queries.
Refactor legacy code to follow modern practices.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I115"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4702,6 +4702,43 @@
         <v>272</v>
       </c>
       <c r="I115" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45902.43356481481</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>0x01,0x10</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>380</v>
+      </c>
+      <c r="G116" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H116" t="n">
+        <v>272</v>
+      </c>
+      <c r="I116" t="n">
         <v>14</v>
       </c>
     </row>
@@ -4716,7 +4753,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I115"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8986,6 +9023,43 @@
         <v>280</v>
       </c>
       <c r="I115" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45902.43356481481</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>0x01,0x14</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>380</v>
+      </c>
+      <c r="G116" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H116" t="n">
+        <v>276</v>
+      </c>
+      <c r="I116" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9000,7 +9074,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I115"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13270,6 +13344,43 @@
         <v>113</v>
       </c>
       <c r="I115" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45902.43356481481</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>0x00,0x71</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>130</v>
+      </c>
+      <c r="G116" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H116" t="n">
+        <v>113</v>
+      </c>
+      <c r="I116" t="n">
         <v>7</v>
       </c>
     </row>
@@ -13284,7 +13395,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I115"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17557,6 +17668,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>45902.43356481481</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>0x00,0x70</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F116" t="n">
+        <v>130</v>
+      </c>
+      <c r="G116" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H116" t="n">
+        <v>112</v>
+      </c>
+      <c r="I116" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add file upload functionality
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4998,6 +4998,117 @@
         <v>264</v>
       </c>
       <c r="I123" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>45910.4328125</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>0x01,0x08</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>380</v>
+      </c>
+      <c r="G124" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H124" t="n">
+        <v>264</v>
+      </c>
+      <c r="I124" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>45911.43440972222</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>0x01,0x08</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>380</v>
+      </c>
+      <c r="G125" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H125" t="n">
+        <v>264</v>
+      </c>
+      <c r="I125" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>45912.43680555555</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>0x01,0x08</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>380</v>
+      </c>
+      <c r="G126" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H126" t="n">
+        <v>264</v>
+      </c>
+      <c r="I126" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5012,7 +5123,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9578,6 +9689,117 @@
         <v>272</v>
       </c>
       <c r="I123" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>45910.4328125</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>0x01,0x10</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>380</v>
+      </c>
+      <c r="G124" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H124" t="n">
+        <v>272</v>
+      </c>
+      <c r="I124" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>45911.43440972222</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>0x01,0x0C</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>380</v>
+      </c>
+      <c r="G125" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H125" t="n">
+        <v>268</v>
+      </c>
+      <c r="I125" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>45912.43680555555</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>0x01,0x0C</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>380</v>
+      </c>
+      <c r="G126" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H126" t="n">
+        <v>268</v>
+      </c>
+      <c r="I126" t="n">
         <v>14</v>
       </c>
     </row>
@@ -9592,7 +9814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14158,6 +14380,117 @@
         <v>112</v>
       </c>
       <c r="I123" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>45910.4328125</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>0x00,0x70</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>130</v>
+      </c>
+      <c r="G124" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H124" t="n">
+        <v>112</v>
+      </c>
+      <c r="I124" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>45911.43440972222</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>0x00,0x70</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>130</v>
+      </c>
+      <c r="G125" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H125" t="n">
+        <v>112</v>
+      </c>
+      <c r="I125" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>45912.43680555555</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>0x00,0x70</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>130</v>
+      </c>
+      <c r="G126" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H126" t="n">
+        <v>112</v>
+      </c>
+      <c r="I126" t="n">
         <v>7</v>
       </c>
     </row>
@@ -14172,7 +14505,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18741,6 +19074,117 @@
         <v>3</v>
       </c>
     </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>45910.4328125</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>0x00,0x6E</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>130</v>
+      </c>
+      <c r="G124" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H124" t="n">
+        <v>110</v>
+      </c>
+      <c r="I124" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>45911.43440972222</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>0x00,0x6E</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>130</v>
+      </c>
+      <c r="G125" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H125" t="n">
+        <v>110</v>
+      </c>
+      <c r="I125" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>45912.43680555555</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>0x00,0x6D</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F126" t="n">
+        <v>130</v>
+      </c>
+      <c r="G126" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H126" t="n">
+        <v>109</v>
+      </c>
+      <c r="I126" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix navigation menu accessibility
Correct null value handling in data processing.
Apply code style fixes as per linter recommendations.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5220,6 +5220,43 @@
         <v>260</v>
       </c>
       <c r="I129" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>45916.43335648148</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>0x01,0x04</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>380</v>
+      </c>
+      <c r="G130" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H130" t="n">
+        <v>260</v>
+      </c>
+      <c r="I130" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5234,7 +5271,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10022,6 +10059,43 @@
         <v>268</v>
       </c>
       <c r="I129" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>45916.43335648148</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>0x01,0x08</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>380</v>
+      </c>
+      <c r="G130" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H130" t="n">
+        <v>264</v>
+      </c>
+      <c r="I130" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10036,7 +10110,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14824,6 +14898,43 @@
         <v>111</v>
       </c>
       <c r="I129" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>45916.43335648148</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>0x00,0x6F</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>130</v>
+      </c>
+      <c r="G130" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H130" t="n">
+        <v>111</v>
+      </c>
+      <c r="I130" t="n">
         <v>7</v>
       </c>
     </row>
@@ -14838,7 +14949,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19629,6 +19740,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>45916.43335648148</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>0x00,0x6D</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F130" t="n">
+        <v>130</v>
+      </c>
+      <c r="G130" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H130" t="n">
+        <v>109</v>
+      </c>
+      <c r="I130" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement config file handling
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5368,6 +5368,43 @@
         <v>256</v>
       </c>
       <c r="I133" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45920.43671296296</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x01,0x00</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>380</v>
+      </c>
+      <c r="G134" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>256</v>
+      </c>
+      <c r="I134" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5382,7 +5419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10318,6 +10355,43 @@
         <v>264</v>
       </c>
       <c r="I133" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45920.43671296296</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x01,0x04</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>380</v>
+      </c>
+      <c r="G134" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>260</v>
+      </c>
+      <c r="I134" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10332,7 +10406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15268,6 +15342,43 @@
         <v>111</v>
       </c>
       <c r="I133" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45920.43671296296</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x00,0x6F</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>130</v>
+      </c>
+      <c r="G134" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>111</v>
+      </c>
+      <c r="I134" t="n">
         <v>7</v>
       </c>
     </row>
@@ -15282,7 +15393,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20221,6 +20332,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>45920.43671296296</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F134" t="n">
+        <v>130</v>
+      </c>
+      <c r="G134" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H134" t="n">
+        <v>108</v>
+      </c>
+      <c r="I134" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize file upload functionality
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5442,6 +5442,43 @@
         <v>256</v>
       </c>
       <c r="I135" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45922.43708333333</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x01,0x00</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>380</v>
+      </c>
+      <c r="G136" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>256</v>
+      </c>
+      <c r="I136" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5456,7 +5493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10466,6 +10503,43 @@
         <v>260</v>
       </c>
       <c r="I135" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45922.43708333333</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x01,0x04</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>380</v>
+      </c>
+      <c r="G136" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>260</v>
+      </c>
+      <c r="I136" t="n">
         <v>14</v>
       </c>
     </row>
@@ -10480,7 +10554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15490,6 +15564,43 @@
         <v>110</v>
       </c>
       <c r="I135" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45922.43708333333</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x00,0x6E</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>130</v>
+      </c>
+      <c r="G136" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>110</v>
+      </c>
+      <c r="I136" t="n">
         <v>7</v>
       </c>
     </row>
@@ -15504,7 +15615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20517,6 +20628,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>45922.43708333333</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F136" t="n">
+        <v>130</v>
+      </c>
+      <c r="G136" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H136" t="n">
+        <v>108</v>
+      </c>
+      <c r="I136" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert api response formatting
Update dependencies to their latest versions.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:I148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5886,6 +5886,43 @@
         <v>240</v>
       </c>
       <c r="I147" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>45934.43471064815</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>0x00,0xF0</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>380</v>
+      </c>
+      <c r="G148" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H148" t="n">
+        <v>240</v>
+      </c>
+      <c r="I148" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5900,7 +5937,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:I148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11354,6 +11391,43 @@
         <v>248</v>
       </c>
       <c r="I147" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>45934.43471064815</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>0x00,0xF8</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>380</v>
+      </c>
+      <c r="G148" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H148" t="n">
+        <v>248</v>
+      </c>
+      <c r="I148" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11368,7 +11442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:I148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16822,6 +16896,43 @@
         <v>108</v>
       </c>
       <c r="I147" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>45934.43471064815</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>130</v>
+      </c>
+      <c r="G148" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H148" t="n">
+        <v>108</v>
+      </c>
+      <c r="I148" t="n">
         <v>7</v>
       </c>
     </row>
@@ -16836,7 +16947,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:I148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22293,6 +22404,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>45934.43471064815</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>0x00,0x69</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F148" t="n">
+        <v>130</v>
+      </c>
+      <c r="G148" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H148" t="n">
+        <v>105</v>
+      </c>
+      <c r="I148" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance api endpoint validation
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I148"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5923,6 +5923,43 @@
         <v>240</v>
       </c>
       <c r="I148" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45935.43868055556</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x00,0xF0</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>380</v>
+      </c>
+      <c r="G149" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>240</v>
+      </c>
+      <c r="I149" t="n">
         <v>14</v>
       </c>
     </row>
@@ -5937,7 +5974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I148"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11428,6 +11465,43 @@
         <v>248</v>
       </c>
       <c r="I148" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45935.43868055556</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x00,0xF4</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>380</v>
+      </c>
+      <c r="G149" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>244</v>
+      </c>
+      <c r="I149" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11442,7 +11516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I148"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16933,6 +17007,43 @@
         <v>108</v>
       </c>
       <c r="I148" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45935.43868055556</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x00,0x6C</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>130</v>
+      </c>
+      <c r="G149" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>108</v>
+      </c>
+      <c r="I149" t="n">
         <v>7</v>
       </c>
     </row>
@@ -16947,7 +17058,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I148"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22441,6 +22552,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>45935.43868055556</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>0x00,0x69</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F149" t="n">
+        <v>130</v>
+      </c>
+      <c r="G149" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H149" t="n">
+        <v>105</v>
+      </c>
+      <c r="I149" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert security vulnerability checks
Fix various typos in comments and documentation.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6071,6 +6071,43 @@
         <v>236</v>
       </c>
       <c r="I152" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>45939.43392361111</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>0x00,0xEC</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>380</v>
+      </c>
+      <c r="G153" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H153" t="n">
+        <v>236</v>
+      </c>
+      <c r="I153" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6085,7 +6122,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11724,6 +11761,43 @@
         <v>244</v>
       </c>
       <c r="I152" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>45939.43392361111</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>0x00,0xF0</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>380</v>
+      </c>
+      <c r="G153" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H153" t="n">
+        <v>240</v>
+      </c>
+      <c r="I153" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11738,7 +11812,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17377,6 +17451,43 @@
         <v>107</v>
       </c>
       <c r="I152" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>45939.43392361111</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>0x00,0x6B</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>130</v>
+      </c>
+      <c r="G153" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H153" t="n">
+        <v>107</v>
+      </c>
+      <c r="I153" t="n">
         <v>7</v>
       </c>
     </row>
@@ -17391,7 +17502,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I152"/>
+  <dimension ref="A1:I153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23033,6 +23144,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>45939.43392361111</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>0x00,0x69</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F153" t="n">
+        <v>130</v>
+      </c>
+      <c r="G153" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H153" t="n">
+        <v>105</v>
+      </c>
+      <c r="I153" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise data parsing logic
Add missing documentation for the new API.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I155"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6182,6 +6182,43 @@
         <v>232</v>
       </c>
       <c r="I155" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="n">
+        <v>45942.43712962963</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>0x00,0xE8</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
+        <v>380</v>
+      </c>
+      <c r="G156" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H156" t="n">
+        <v>232</v>
+      </c>
+      <c r="I156" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6196,7 +6233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I155"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11946,6 +11983,43 @@
         <v>240</v>
       </c>
       <c r="I155" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="n">
+        <v>45942.43712962963</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>0x00,0xF0</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
+        <v>380</v>
+      </c>
+      <c r="G156" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H156" t="n">
+        <v>240</v>
+      </c>
+      <c r="I156" t="n">
         <v>14</v>
       </c>
     </row>
@@ -11960,7 +12034,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I155"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17710,6 +17784,43 @@
         <v>107</v>
       </c>
       <c r="I155" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="n">
+        <v>45942.43712962963</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>0x00,0x6B</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
+        <v>130</v>
+      </c>
+      <c r="G156" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H156" t="n">
+        <v>107</v>
+      </c>
+      <c r="I156" t="n">
         <v>7</v>
       </c>
     </row>
@@ -17724,7 +17835,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I155"/>
+  <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23477,6 +23588,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="156">
+      <c r="A156" s="2" t="n">
+        <v>45942.43712962963</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>0x00,0x68</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F156" t="n">
+        <v>130</v>
+      </c>
+      <c r="G156" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H156" t="n">
+        <v>104</v>
+      </c>
+      <c r="I156" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance error message display
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6256,6 +6256,43 @@
         <v>232</v>
       </c>
       <c r="I157" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45944.43943287037</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x00,0xE8</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>380</v>
+      </c>
+      <c r="G158" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>232</v>
+      </c>
+      <c r="I158" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6270,7 +6307,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12094,6 +12131,43 @@
         <v>240</v>
       </c>
       <c r="I157" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45944.43943287037</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x00,0xEC</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>380</v>
+      </c>
+      <c r="G158" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>236</v>
+      </c>
+      <c r="I158" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12108,7 +12182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17932,6 +18006,43 @@
         <v>107</v>
       </c>
       <c r="I157" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45944.43943287037</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x00,0x6A</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>130</v>
+      </c>
+      <c r="G158" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>106</v>
+      </c>
+      <c r="I158" t="n">
         <v>7</v>
       </c>
     </row>
@@ -17946,7 +18057,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I157"/>
+  <dimension ref="A1:I158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23773,6 +23884,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>45944.43943287037</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>0x00,0x68</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F158" t="n">
+        <v>130</v>
+      </c>
+      <c r="G158" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H158" t="n">
+        <v>104</v>
+      </c>
+      <c r="I158" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement logging system configuration
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6478,6 +6478,43 @@
         <v>224</v>
       </c>
       <c r="I163" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>45950.43614583334</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>0x00,0xDC</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>380</v>
+      </c>
+      <c r="G164" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H164" t="n">
+        <v>220</v>
+      </c>
+      <c r="I164" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6492,7 +6529,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12538,6 +12575,43 @@
         <v>232</v>
       </c>
       <c r="I163" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>45950.43614583334</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>0x00,0xE8</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>380</v>
+      </c>
+      <c r="G164" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H164" t="n">
+        <v>232</v>
+      </c>
+      <c r="I164" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12552,7 +12626,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18598,6 +18672,43 @@
         <v>106</v>
       </c>
       <c r="I163" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>45950.43614583334</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>0x00,0x6A</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>130</v>
+      </c>
+      <c r="G164" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H164" t="n">
+        <v>106</v>
+      </c>
+      <c r="I164" t="n">
         <v>7</v>
       </c>
     </row>
@@ -18612,7 +18723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24661,6 +24772,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>45950.43614583334</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>0x00,0x67</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F164" t="n">
+        <v>130</v>
+      </c>
+      <c r="G164" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H164" t="n">
+        <v>103</v>
+      </c>
+      <c r="I164" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert database schema migration
This resolves issue #83.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6552,6 +6552,43 @@
         <v>220</v>
       </c>
       <c r="I165" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45952.43814814815</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>0x00,0xDC</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>380</v>
+      </c>
+      <c r="G166" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H166" t="n">
+        <v>220</v>
+      </c>
+      <c r="I166" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6566,7 +6603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12686,6 +12723,43 @@
         <v>228</v>
       </c>
       <c r="I165" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45952.43814814815</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>0x00,0xE4</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>380</v>
+      </c>
+      <c r="G166" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H166" t="n">
+        <v>228</v>
+      </c>
+      <c r="I166" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12700,7 +12774,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18820,6 +18894,43 @@
         <v>106</v>
       </c>
       <c r="I165" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45952.43814814815</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>0x00,0x69</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>130</v>
+      </c>
+      <c r="G166" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H166" t="n">
+        <v>105</v>
+      </c>
+      <c r="I166" t="n">
         <v>7</v>
       </c>
     </row>
@@ -18834,7 +18945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24957,6 +25068,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>45952.43814814815</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>0x00,0x67</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F166" t="n">
+        <v>130</v>
+      </c>
+      <c r="G166" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H166" t="n">
+        <v>103</v>
+      </c>
+      <c r="I166" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimize api response formatting
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6589,6 +6589,43 @@
         <v>220</v>
       </c>
       <c r="I166" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45953.43768518518</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x00,0xDC</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>380</v>
+      </c>
+      <c r="G167" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>220</v>
+      </c>
+      <c r="I167" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6603,7 +6640,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12760,6 +12797,43 @@
         <v>228</v>
       </c>
       <c r="I166" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45953.43768518518</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x00,0xE0</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>380</v>
+      </c>
+      <c r="G167" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>224</v>
+      </c>
+      <c r="I167" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12774,7 +12848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18931,6 +19005,43 @@
         <v>105</v>
       </c>
       <c r="I166" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45953.43768518518</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x00,0x69</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>130</v>
+      </c>
+      <c r="G167" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>105</v>
+      </c>
+      <c r="I167" t="n">
         <v>7</v>
       </c>
     </row>
@@ -18945,7 +19056,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25105,6 +25216,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>45953.43768518518</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>0x00,0x67</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F167" t="n">
+        <v>130</v>
+      </c>
+      <c r="G167" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H167" t="n">
+        <v>103</v>
+      </c>
+      <c r="I167" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix security vulnerability checks
Refactor legacy code to follow modern practices.
Remove deprecated functions and clean up codebase.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I168"/>
+  <dimension ref="A1:I169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6663,6 +6663,43 @@
         <v>216</v>
       </c>
       <c r="I168" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>45955.43486111111</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>0x00,0xD8</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F169" t="n">
+        <v>380</v>
+      </c>
+      <c r="G169" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H169" t="n">
+        <v>216</v>
+      </c>
+      <c r="I169" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6677,7 +6714,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I168"/>
+  <dimension ref="A1:I169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12908,6 +12945,43 @@
         <v>224</v>
       </c>
       <c r="I168" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>45955.43486111111</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>0x00,0xE0</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F169" t="n">
+        <v>380</v>
+      </c>
+      <c r="G169" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H169" t="n">
+        <v>224</v>
+      </c>
+      <c r="I169" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12922,7 +12996,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I168"/>
+  <dimension ref="A1:I169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19153,6 +19227,43 @@
         <v>105</v>
       </c>
       <c r="I168" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>45955.43486111111</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>0x00,0x68</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F169" t="n">
+        <v>130</v>
+      </c>
+      <c r="G169" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H169" t="n">
+        <v>104</v>
+      </c>
+      <c r="I169" t="n">
         <v>7</v>
       </c>
     </row>
@@ -19167,7 +19278,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I168"/>
+  <dimension ref="A1:I169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25401,6 +25512,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>45955.43486111111</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>0x00,0x66</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F169" t="n">
+        <v>130</v>
+      </c>
+      <c r="G169" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H169" t="n">
+        <v>102</v>
+      </c>
+      <c r="I169" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert error message display
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I169"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6700,6 +6700,43 @@
         <v>216</v>
       </c>
       <c r="I169" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>45956.43445601852</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>0x00,0xD8</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F170" t="n">
+        <v>380</v>
+      </c>
+      <c r="G170" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H170" t="n">
+        <v>216</v>
+      </c>
+      <c r="I170" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6714,7 +6751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I169"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12982,6 +13019,43 @@
         <v>224</v>
       </c>
       <c r="I169" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>45956.43445601852</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>0x00,0xE0</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F170" t="n">
+        <v>380</v>
+      </c>
+      <c r="G170" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H170" t="n">
+        <v>224</v>
+      </c>
+      <c r="I170" t="n">
         <v>14</v>
       </c>
     </row>
@@ -12996,7 +13070,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I169"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19264,6 +19338,43 @@
         <v>104</v>
       </c>
       <c r="I169" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>45956.43445601852</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>0x00,0x68</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F170" t="n">
+        <v>130</v>
+      </c>
+      <c r="G170" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H170" t="n">
+        <v>104</v>
+      </c>
+      <c r="I170" t="n">
         <v>7</v>
       </c>
     </row>
@@ -19278,7 +19389,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I169"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25549,6 +25660,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>45956.43445601852</v>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>0x00,0x65</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F170" t="n">
+        <v>130</v>
+      </c>
+      <c r="G170" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H170" t="n">
+        <v>101</v>
+      </c>
+      <c r="I170" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Simplify unit test coverage
Enhance test coverage to prevent regressions.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I174"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6885,6 +6885,43 @@
         <v>212</v>
       </c>
       <c r="I174" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>45961.43393518519</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>0x00,0xD4</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F175" t="n">
+        <v>380</v>
+      </c>
+      <c r="G175" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H175" t="n">
+        <v>212</v>
+      </c>
+      <c r="I175" t="n">
         <v>14</v>
       </c>
     </row>
@@ -6899,7 +6936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I174"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13352,6 +13389,43 @@
         <v>220</v>
       </c>
       <c r="I174" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>45961.43393518519</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>0x00,0xDC</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F175" t="n">
+        <v>380</v>
+      </c>
+      <c r="G175" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H175" t="n">
+        <v>220</v>
+      </c>
+      <c r="I175" t="n">
         <v>14</v>
       </c>
     </row>
@@ -13366,7 +13440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I174"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19819,6 +19893,43 @@
         <v>103</v>
       </c>
       <c r="I174" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>45961.43393518519</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>0x00,0x67</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F175" t="n">
+        <v>130</v>
+      </c>
+      <c r="G175" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H175" t="n">
+        <v>103</v>
+      </c>
+      <c r="I175" t="n">
         <v>7</v>
       </c>
     </row>
@@ -19833,7 +19944,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I174"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26289,6 +26400,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>45961.43393518519</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>0x00,0x64</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F175" t="n">
+        <v>130</v>
+      </c>
+      <c r="G175" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H175" t="n">
+        <v>100</v>
+      </c>
+      <c r="I175" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update error message display
This resolves issue #74.
Add input validation for better security.
</commit_message>
<xml_diff>
--- a/DE2025May_Database_update.xlsx
+++ b/DE2025May_Database_update.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I178"/>
+  <dimension ref="A1:I179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7033,6 +7033,43 @@
         <v>208</v>
       </c>
       <c r="I178" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>45965.43454861111</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x46,0x93,0x3c,0x23,0x3f,0x43,0xe8,0xa0,</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>0x00,0xD0</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>0x14</t>
+        </is>
+      </c>
+      <c r="F179" t="n">
+        <v>380</v>
+      </c>
+      <c r="G179" t="n">
+        <v>7.598631275147109e+23</v>
+      </c>
+      <c r="H179" t="n">
+        <v>208</v>
+      </c>
+      <c r="I179" t="n">
         <v>14</v>
       </c>
     </row>
@@ -7047,7 +7084,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I178"/>
+  <dimension ref="A1:I179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13648,6 +13685,43 @@
         <v>216</v>
       </c>
       <c r="I178" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>45965.43454861111</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>0x01,0x7c</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>0x00,0xa6,0x60,0x33,0x96,0x39,0x62,0xd0,0x5e,0x78,</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>0x00,0xD8</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>0xe</t>
+        </is>
+      </c>
+      <c r="F179" t="n">
+        <v>380</v>
+      </c>
+      <c r="G179" t="n">
+        <v>5.68432987514711e+23</v>
+      </c>
+      <c r="H179" t="n">
+        <v>216</v>
+      </c>
+      <c r="I179" t="n">
         <v>14</v>
       </c>
     </row>
@@ -13662,7 +13736,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I178"/>
+  <dimension ref="A1:I179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20263,6 +20337,43 @@
         <v>103</v>
       </c>
       <c r="I178" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>45965.43454861111</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>0x78,0x69,0x90,0x01,0x00,0x00,0x18,0x0b,0x40,0x0c,</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>0x00,0x67</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>0x7</t>
+        </is>
+      </c>
+      <c r="F179" t="n">
+        <v>130</v>
+      </c>
+      <c r="G179" t="n">
+        <v>5.68631262647114e+23</v>
+      </c>
+      <c r="H179" t="n">
+        <v>103</v>
+      </c>
+      <c r="I179" t="n">
         <v>7</v>
       </c>
     </row>
@@ -20277,7 +20388,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I178"/>
+  <dimension ref="A1:I179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26881,6 +26992,43 @@
         <v>3</v>
       </c>
     </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>45965.43454861111</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>0x00,0x82</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>0xd0,0x97,0x78,0x01,0x00,0x00,0x0e,0x3f,0x0c,0x0c,</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>0x00,0x64</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>0x3</t>
+        </is>
+      </c>
+      <c r="F179" t="n">
+        <v>130</v>
+      </c>
+      <c r="G179" t="n">
+        <v>9.85046333984776e+23</v>
+      </c>
+      <c r="H179" t="n">
+        <v>100</v>
+      </c>
+      <c r="I179" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>